<commit_message>
making paypal callback, not working, to be continued
</commit_message>
<xml_diff>
--- a/doc/GDS_Batch_Order.xlsx
+++ b/doc/GDS_Batch_Order.xlsx
@@ -125,8 +125,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -156,7 +158,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -168,6 +170,7 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -179,6 +182,7 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -511,7 +515,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
to debug paypal callback
</commit_message>
<xml_diff>
--- a/doc/GDS_Batch_Order.xlsx
+++ b/doc/GDS_Batch_Order.xlsx
@@ -515,7 +515,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -559,7 +559,7 @@
         <v>13579</v>
       </c>
       <c r="B2">
-        <v>1501</v>
+        <v>100065</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -588,7 +588,7 @@
         <v>13579</v>
       </c>
       <c r="B3">
-        <v>1501</v>
+        <v>100065</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -617,7 +617,7 @@
         <v>24680</v>
       </c>
       <c r="B4">
-        <v>1501</v>
+        <v>100065</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -666,7 +666,7 @@
         <v>13579</v>
       </c>
       <c r="B10">
-        <v>1501</v>
+        <v>100065</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -695,7 +695,7 @@
         <v>13579</v>
       </c>
       <c r="B11">
-        <v>1501</v>
+        <v>100065</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -724,7 +724,7 @@
         <v>24680</v>
       </c>
       <c r="B12">
-        <v>1501</v>
+        <v>100065</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>

</xml_diff>